<commit_message>
fix minor bug. backup for further changes
</commit_message>
<xml_diff>
--- a/account/link_account.xlsx
+++ b/account/link_account.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$C$31</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$C$107</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,199 +448,199 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tra chanh</t>
+          <t>hardcore1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=voreios2412@goid&amp;pass=47b342d262e17dc91ee72387a21e2a71&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>main</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>nuoc suoi</t>
+          <t>hardcore2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=huyhoang0710@goid&amp;pass=fe6cce52c505e12db0acdf8b350fbde9&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>main</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>bac siu</t>
+          <t>hardcore3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=sanatori@goid&amp;pass=13d0c9cc0a0e56ce39bca83b31aea91c&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>main</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>tra tac</t>
+          <t>hardcore4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=nhoctin12@goid&amp;pass=a333caabb313195bd5f06fcd2f0700ab&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>main</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>anh vi ca</t>
+          <t>hardcore5</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoader.swf?user=babys0beiu&amp;pass=1713b88af3f969dfd2ca4416a9060567&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>main</t>
+          <t>trainquang1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>comeback1</t>
+          <t>hardcore5</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=comeback1@goid&amp;pass=eb0e4ab7049c9f6c6640b2856577f0d9&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>comeback</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>comeback2</t>
+          <t>hardcore1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=comeback2@goid&amp;pass=c51cfbc05d9f20661d27f083349a5e23&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>comeback</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>comeback3</t>
+          <t>hardcore2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=comeback3@goid&amp;pass=e3435f6c043051e3418eed0980d31e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>comeback</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>comeback4</t>
+          <t>hardcore3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=comeback4@goid&amp;pass=abc5173543565271692ed4bf0b720c38&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>comeback</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>comeback5</t>
+          <t>hardcore4</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=comeback5@goid&amp;pass=42e8657699a54e42d8a137ffe8e83bf7&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>comeback</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>hardcore1</t>
+          <t>hardcore5</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>hardcore</t>
+          <t>trainquang1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>hardcore2</t>
+          <t>hardcore5</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -652,29 +652,29 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>hardcore3</t>
+          <t>hardcore5</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>hardcore</t>
+          <t>trainquang2</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>hardcore4</t>
+          <t>hardcore1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -686,12 +686,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>hardcore5</t>
+          <t>hardcore2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -703,260 +703,1544 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>lazyas01</t>
+          <t>hardcore3</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=lazyas01@goid&amp;pass=4f26d07de6091c053539c1961e2f28d3&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>lazyas</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>lazyas02</t>
+          <t>hardcore4</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=lazyas02@goid&amp;pass=144cb9dc639a5f650ac8a55210f6a4e0&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>lazyas</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>lazyas03</t>
+          <t>hardcore5</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=lazyas03@goid&amp;pass=f0d561300549681c658526e81295e35d&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>lazyas</t>
+          <t>trainquang1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>lazyas04</t>
+          <t>hardcore5</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=lazyas04@goid&amp;pass=1d05b0856a70efc0a72edaecdd0c1380&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>lazyas</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>lazyas05</t>
+          <t>hardcore1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=lazyas05@goid&amp;pass=4594ea462f046e947a593ace166f38e1&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>lazyas</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>honda01</t>
+          <t>hardcore2</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=honda01@goid&amp;pass=3022be2cc095883b5d3f4a067edd353e&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>honda</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>honda02</t>
+          <t>hardcore3</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=honda02@goid&amp;pass=336417a421a018a8bd6654b4f09ff2a2&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>honda</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>honda03</t>
+          <t>hardcore4</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=honda03@goid&amp;pass=cd494251f85f81fcd039849e0b3fa31b&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>honda</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>honda04</t>
+          <t>hardcore5</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=honda04@goid&amp;pass=bb58e8aeed4d5447c5b3e01ea0edb87c&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>honda</t>
+          <t>trainquang1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>honda05</t>
+          <t>hardcore5</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=honda05@goid&amp;pass=63ae498c4c94859b204eb71a08c72345&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>honda</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>antham1</t>
+          <t>hardcore5</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=antham1@goid&amp;pass=25b98999ec78b7243b282875e64f2d38&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>antham</t>
+          <t>trainquang2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>antham2</t>
+          <t>hardcore1</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=antham2@goid&amp;pass=f8ae8256508a4523c95bde1319158793&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>antham</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>antham3</t>
+          <t>hardcore2</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=antham3@goid&amp;pass=ebf3132817ba8040a49689cc3cf56268&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>antham</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>antham4</t>
+          <t>hardcore3</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=antham4@goid&amp;pass=6ec6aedf0e19bee10073a9fb98b2010c&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>antham</t>
+          <t>hardcore</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>antham5</t>
+          <t>hardcore4</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=antham5@goid&amp;pass=154eb502414ed8c5acb5220eeb272ea2&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>antham</t>
-        </is>
-      </c>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>hardcore1</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>hardcore2</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>hardcore3</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>hardcore4</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>trainquang2</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>hardcore1</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>hardcore2</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>hardcore3</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>hardcore4</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>hardcore1</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>hardcore2</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>hardcore3</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>hardcore4</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>trainquang2</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>hardcore1</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>hardcore2</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>hardcore3</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>hardcore4</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>hardcore1</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>hardcore2</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>hardcore3</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>hardcore4</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>trainquang2</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>hardcore1</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>hardcore2</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>hardcore3</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>hardcore4</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>hardcore1</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>hardcore2</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>hardcore3</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>hardcore4</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>trainquang2</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>hardcore1</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>hardcore2</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>hardcore3</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>hardcore4</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>hardcore1</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>hardcore2</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>hardcore3</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>hardcore4</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>trainquang2</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>hardcore1</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>hardcore2</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>hardcore3</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>hardcore4</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>hardcore1</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore1@goid&amp;pass=57eb28cbdd0056c78044e36aafac9bad&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>hardcore2</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore2@goid&amp;pass=0248a0c0e0125dc6b8ca3ad38c588ad8&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>hardcore3</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore3@goid&amp;pass=ffbce798336a35e812c7f06358eb76b4&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>hardcore4</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore4@goid&amp;pass=06f9cda927d0bb95a8c483d75c6f1735&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>trainquang1</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>hardcore</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>hardcore5</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>http://s3.vuaphapthuat.goplay.vn/s/s40/GameLoaders.swf?user=hardcore5@goid&amp;pass=3e3872776ceea81ceb76206076749e59&amp;version=0.9.9a33.271&amp;isExpand=true</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>trainquang2</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>12312</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>12312</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>xcvxzcv</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>sdfasd</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C31"/>
+  <autoFilter ref="A1:C107"/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>